<commit_message>
Se permite comparar archivos XLSX
- Se utiliza FilePicker para seleccionar archivo del dispositivo.
- Se usa paquete ClosedXML para trabajar con archivos XLSX.
- Se utiliza FileSystem.AppDataDirectory para obtener la ruta donde guardar archivos de la aplicación.
- Se utiliza Share para compartir archivo generado.
</commit_message>
<xml_diff>
--- a/Tests/file1.xlsx
+++ b/Tests/file1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bogotá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neiva</t>
   </si>
 </sst>
 </file>
@@ -73,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -132,8 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,67 +271,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>